<commit_message>
Get daily reddit data: Tue Mar 18 08:11:42 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_23.xlsx
+++ b/data/collected_data/2025_03_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C519"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3712 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1jdznz9</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Treated myself with new nails on my birthday💅</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5o8ujd5kepe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1jdyi74</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Obsessed with this red cat eye 🍒</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdge767u3epe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1jdy94v</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Spring nails 🌱🌷</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxhfl9em0epe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1jdy7n9</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Was short almond a mistake?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdy7n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1jdy27m</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Do my nails look dumb?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdy27m</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1jdxrkp</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>I just turned 27 and decided to make my own set of birthday nails.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdxrkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1jdv974</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>got flamed for these on tiktok, how can i improve?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdv974</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1jdv3yo</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>St. Paddy’s Day nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdv3yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1jdx5yj</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>I always have to be extra 💅</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5jwyys9dndpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1jdwzpf</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>How can I make sure my nails don’t break and keep growing</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdwzpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1jdwre1</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Ancient Greek pottery set</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl6ogknuidpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1jdwpec</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Reasonable Costs</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdwpec/reasonable_costs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1jdwajo</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Please help</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wst3lxpyddpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1jdvt8y</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Smoothed and shined my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdvt8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1jdvrzm</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Scarab vibes</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnsh2xau8dpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1jdvf4d</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>First time making my own press on nails ☺️</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdvf4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1jdvdz1</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Got SNS for the first time</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdvdz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1jdvcjw</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>27th Birthday Set 💅🏻🐆🥰</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdvcjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1jdv70v</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk4di05c3dpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1jduxq9</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>in love</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7u3k7b4y0dpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1jdsu7l</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>How do I know what kind of nails to get?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdsu7l/how_do_i_know_what_kind_of_nails_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1jdtkcc</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Will my nail tech be able to add a tip to this nail?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwtb1xfnocpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1jdueff</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>My 🍓 Nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdueff</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1jdu3g3</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Another set complete!</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izfkh5katcpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1jdtvoa</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Birthday/St Patrick’s day nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21atshqercpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1jdttq4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>How do y’all get such good pics of your nails?? Mine look like my hand is getting a DUI mugshot 😫</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdttq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1jdtjvg</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>finally managed to sculpt a decent 3d flower :)!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdtjvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1jdtizf</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>St. Paddy's nails! 2 hands, 2 different vibes lol</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdtizf</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1jdtht8</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Teal and purple cat eye</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdtht8</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1jdt42z</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Gold chrome design has been my everything lately!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq5fhx0pkcpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1jdt201</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Aura nails</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdt201</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1jdsz6t</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Spring is here🍀</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y3dde5ijcpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1jdsyz4</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Decided to change my nail shape after 15 years. Almond vs Coffin</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdsyz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1jdswap</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>🎀 🍬 Candy Pink 🍬 🎀 to meet my boyfriend’s family for the first time!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v29z8xzsicpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1jdsusf</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>White because spring is almost here🤍🌸</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9zcimzficpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1jdssuz</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Love my new set!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdssuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1jdsb2p</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdsb2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1jdschk</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Spring nails 🎀💅🏼</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqqtlsw1ecpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1jds60d</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Fastest way to do nails?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jds60d/fastest_way_to_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1jds50e</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Random gift from my little sis ❤️</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fphken9ccpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1jdrzvn</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I don't know why I chose gold, immediate regret lol</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9as8a9u3bcpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1jdryok</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Back to my favorite icy pink nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdryok</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1jdrw7z</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I did my sister’s nails ❤️</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e19m3s4aacpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1jdrvuk</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Prettiest nails I've ever done</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3paww267acpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1jdrm6q</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Best nails I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdrm6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1jdri6t</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>My recent set (and my go-to color!)</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yecbky227cpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1jdr7ch</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>nail sets from the past year!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdr7ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1jdqsud</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Glamnetics Love</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9odwr5bc1cpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1jdqx1v</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Tortoise shell and bright colors for my birthday 🐢💕</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdqx1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1jdqm4b</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Soap nails lmao get it haha we have fun here</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd0d2nnvzbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1jdq5dp</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Natural Nail Tips?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdq5dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1jdpwtk</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>goth nails but make them ✨</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xex1mivbubpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1jdpmin</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>These are so cute</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34xzgkn3sbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1jdp025</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>natural nails after 2 months of BIAB 🫶🏽</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3y5x3vbnbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1jdorxc</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Newest Sets</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdorxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1jdolct</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Love a french cat eye~ 🩰🫧</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5zow1ak7kbpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1jdo93s</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Fruits, florals, or animal?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdd85glohbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1jdntvm</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Love me some white glitter :)</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xddc7kumebpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1jdnoyf</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Pink Flamenco to welcome warmer weather!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2bxk9gndbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1jdnc7o</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Glow crackle st paddy's day set</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdnc7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1jdmoyw</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Favorite hacks for not breaking a nail</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdmoyw/favorite_hacks_for_not_breaking_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1jdmsjw</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>What does it mean when your nails cause you pain after you get acrylics?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdmsjw/what_does_it_mean_when_your_nails_cause_you_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1jdn5xb</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Missing big nails! 😕</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdn5xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1jdn4he</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>How could i make improvements?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdn4he</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1jdn2ub</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>New nails - but that left pinky. The base is narrow, right?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdn2ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1jdn108</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Howls Moving Castle themed nails I got off etsy (BlancNail)</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgwcq66u8bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1jdn0t5</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>How many nails broken before you trim the rest down?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdn0t5/how_many_nails_broken_before_you_trim_the_rest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1jdmf6h</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>split nail hellllp</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdmf6h/split_nail_hellllp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1jdmguc</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>So shinyyy</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdmguc</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1jdmfir</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Are these grown out looking?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdmfir</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1jdmfi5</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>First time trying red press-ons! ❤️</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ahqerfi4bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1jdm9zm</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Press ons are so underrated!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0ruehhf3bpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1jdlys3</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Looking for Dupe !!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdlys3</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1jdlhwj</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Why is it that all the gel nail colours set on Amazon are all 5ml bottles?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdlhwj/why_is_it_that_all_the_gel_nail_colours_set_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1jdl5zv</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>My 2nd attempt at acrylic</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo6ffvmgvape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1jdktdi</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Pinkie nails have a defect and grow like this- any good solutions?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3ztz8xzsape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1jdkwho</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Simple and clean</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr8i9vrktape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1jdkt6g</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>How to change c curve?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdkt6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1jdkqrf</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Baddie nails</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epql4odhsape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1jdknk9</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Lucky charms St Patty's Day nails</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdknk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1jdki5r</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Beautiful futuristic desing</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecp5unouqape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1jdkhvr</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Went to a new nail salon for the 1st time</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdkhvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1jdke4m</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Suggest a nude color.</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4qnvmg1qape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1jdkdka</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Wearing at edge of nail even though it’s only been 2 days? (Gel)</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdkdka</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1jdk9ze</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Longest nails I ever had!</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20uuak49pape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1jdk3o2</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Learning to do my own GelX nails - Advice please :)</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p8ou0fznape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1jdjvfk</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Life hack for protecting your nails from those pesky key rings: staple remover to the rescue!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bf2xudjcmape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1jdjtae</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>St. Paddy’s Mani!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdjtae</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1jdjib5</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Uv Gel set vs gel manicure</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdjib5/uv_gel_set_vs_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1jdirgv</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>my newest set 🤎</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5yimy5keape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1jdijry</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>First time doing a design on my nails. Happy with results. Super basic design</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z5f2gu0dape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1jdi4xl</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Any idea on what’s going on</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w765e7r3aape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1jdi5ou</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Best drill bits for dry manicure?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hii5zq8aape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1jdeen9</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Advice please on what happened to my nail</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdeen9</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1jdhykt</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Nail tech not answering, nails lifting , no answer , soak off?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jdhykt/nail_tech_not_answering_nails_lifting_no_answer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1jdgbto</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Experiment goes RIGHT 💅🏽</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdgbto</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1jdb0g1</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Messed up nails</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vckk15wp8pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1jddlvj</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>How do I stop my nails from looking like THIS!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jddlvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1jdhsaz</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Clean and Fresh</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdhsaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1jdgogc</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Are my nails over filed? 😭</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qifrt5wrz9pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1jdzxmi</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Rainbow 🌈 mani</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13pg9nf1oepe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1jdy310</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Just a mom finding herself after postpartum…</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zv0hg3gfydpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1jdy0u3</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Blues and Greens</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ta551z2nxdpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1jdxp7s</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Heard we are doing green and gold.</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdxp7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1jdxgpp</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Happy St. Patrick's Day!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdxgpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1jdx9so</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Made a wheel of [nail polish] fortune tonight for those days that I’m extremely indecisive</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04clxf3modpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1jdx9n8</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Has anyone seen this?? Need to watch it</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du772m8kodpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1jdwxvl</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Peeling Nails</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdwxvl/peeling_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1jduuy9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Has anyone used nail stamps?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jduuy9/has_anyone_used_nail_stamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1jdupb4</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Dupe recommendations??</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nt2my6tycpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1jdu72v</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Advice on working with Holo Taco Garden Party?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdu72v/advice_on_working_with_holo_taco_garden_party/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1jdtu3s</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>🍀 At the End of the Rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdtu3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1jdtkcu</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>When hobbies collide ☘️</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdtkcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1jdtegl</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>French Nail Stickers</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdtegl/french_nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1jdstuz</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Is there a regular polish dupe for this shellac shade?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdstuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1jdsbnw</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Looking for thermals shipping from within (from and to) Canada :)</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdsbnw/looking_for_thermals_shipping_from_within_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1jds63e</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Lucky Charms 🍀💞</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jds63e</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1jds2xz</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Happy St Paddy’s Day!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jds2xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1jdrfv3</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>one of my favorites 💙</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdrfv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1jdqurp</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>My St Paddy's contribution</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdqurp</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1jdqngw</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>First time I've applied this powder. My nails look metallic and scream rock.</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if4lhag40cpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1jdqbw6</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Finally caved and painted them green☘️</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdqbw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1jdq4bi</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Tomorrow I'll call them spring nails</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hit05byvbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1jdpwbp</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>No pinches for me today!</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pekx6g67ubpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1jdplh7</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>A little pearly shine on an overcast day💖</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsrucksvrbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1jdpi8f</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Happy St. Patrick’s Day!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwphrv87rbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1jdpdak</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Press on nails break time</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdpdak/press_on_nails_break_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1jdpavu</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Mooncat Serpents of Eden is perfect for St. Paddy's Day and I can still see my favorite color in it (blue)!</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wyf5lusmpbpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1jdp08o</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>HT existential crisis vs MC am I everything you fear?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdp08o/ht_existential_crisis_vs_mc_am_i_everything_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1jdovf2</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>I’ve been saving this one for St. Patrick’s Day but it’s also giving Christmas</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdovf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1jdosa8</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Here to beg for assistance again 🙏🏼💅🏻</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82hmlzrnlbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1jdofe9</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Unintentional ApocalypseNnails for St. Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdofe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1jdo7rs</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Yes, that's a potato.</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/376eojiehbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1jdo7dz</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Pixie party+Gummy bear!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdo7dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1jdo0sk</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Uv resin ingredient</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdo0sk/uv_resin_ingredient/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1jdo0lm</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Holo Taco “Orange Drink”</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd2aj8fyfbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1jdnpai</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Anyone else have their nails start splitting or flaking from ridge filling base coats?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdnpai</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1jdnnm8</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>🍀St Paddy's glow crackle set🍀</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdnnm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1jdnf1u</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Dreamy set</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7leyxvfobbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1jdnd6u</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Lucky Charms? (Blowin Bubbles)</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdnd6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1jdnbmz</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Had a cool idea, but not sure it translated well</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdnbmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1jdn5mt</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>🌸🦄🌸</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zxnljh8zape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1jdn2ul</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Hi! Can anyone help me find this green or similar? Preferably something I can buy on Amazon.</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7meax2f79bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1jdmrky</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Mooncat primers and top coats?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdmrky/mooncat_primers_and_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1jdmpuy</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>My nails look...tasty?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdmpuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1jdmj6s</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>[ISO] Neon green/teal base with blue/aqua shimmer</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdmj6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1jdm6w0</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Little shade comparison</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xm422mcu2bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1jdm5wp</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Obsessed with this glow ✨</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c40igtn2bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1jdm2fl</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>St. Patrick’s Day Mani 2025 🍀</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp1uxydy1bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1jdlox4</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Easter mani</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdlox4</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1jdlhym</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Mansfield Park💚</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdlhym</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1jdl1in</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>do you wear gloves in the shower?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdl1in/do_you_wear_gloves_in_the_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1jdktyn</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>A somewhat bizarre St. Paddy's Day Mani 💚</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0shgt14tape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1jdkmvu</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>My February PPU order was pretty green.</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdkmvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1jdjymg</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Didn't want to get pinched!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9ho80nzmape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1jdjwiz</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Happy St. Patrick’s Day! 💚</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwe7w4rkmape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1jdjk8a</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Lucky green!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdjk8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1jdjamh</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>just a warning for those of you who have Death Valley Nails!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdjamh/just_a_warning_for_those_of_you_who_have_death/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1jdj9qm</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Best single color magnetics? like ILNP Poison. Meaning no shift in magnetic pigment. Need green and gold in particular</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdj9qm/best_single_color_magnetics_like_ilnp_poison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1jdj2tn</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>“One size fits all” blurring base?</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdj2tn/one_size_fits_all_blurring_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1jdix27</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Sparkling St Patrick’s Day Green</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cxeuy7nfape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1jdipu6</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Mooncat Fields of Lavender Velvet</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/js2e3oi7eape1</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1jdhrjp</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Bright colors and tortoise shell for my birthday set 🐢💕</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdhrjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1jdhffg</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Finally Sunny Enough to Show Off Some Holo!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i81czq465ape1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1jdh0rx</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>ILNP: Chai Latte</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdh0rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1jdh0ke</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>I heard we were showing off our shadow realms polish?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gcx9vz52ape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1jdgxbe</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Absolutely love these files. I have a Pedicure file coming too. 3mm thick (unlike some brands) and works so well. Looking forward to a long long time with them. 👍🏼👍🏼</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gq2s5uh1ape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1jdgwmv</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Looking for a buttery yellow for spring!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdgwmv/looking_for_a_buttery_yellow_for_spring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1jdgsr5</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Cadillaquer - Hiding From The Real World</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdgsr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1jdgrgb</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>St. Pattys Day Chaos Mani 🍀</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdgrgb</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1jdg5v5</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Can anyone help me ID this polish?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cth0oth3w9pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1jdfk6r</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Why is my nail bending like this?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mycpkirr9pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1jdf3fb</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Last minute green 🍀</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdf3fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1jdevq7</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>My reflection is wearing a completely different color than me lol</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej4rkd0sm9pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1jderl6</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>I can see why it’s so beloved</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jtm12jjwl9pe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1jdek3g</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Mooncat Castle of Cobwebs</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdek3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1jde1sd</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>A work of art and captivating “neutral” 🍂❤️</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jde1sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1jddty8</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jddty8</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1jddlqf</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>🌈🍀Another St. Patrick's Mani🍀🌈</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jddlqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1jddk5s</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I gave myself the most obnoxious manicure for St. Paddy's Day</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jddk5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1jdd3k7</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Fawning over Fawn</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ye6bulmr89pe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1jdcvbl</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>matching the pickle balls 🎾</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdcvbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1jdciad</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>…And Fire🧲❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdciad</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1jdcdeo</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Can't stop staring</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdcdeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1jdbqgb</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Frist time trying pearl powder</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5779ymwxw8pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1jdabx5</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Beautiful spring days are coming!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr0n64dqi8pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1jdaaru</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>lucky little rainbows 🌈</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdaaru</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1jd9gfz</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Chemical X 🖤🧪</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu1m0xwr88pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1jd92su</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jd92su/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1jd8hzo</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Decided to welcome spring time with something bright. Happy St Patrick’s Day!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jd8hzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1jcmjnh</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Less milky and pink sheer nude recommendations for a naked french manicure?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jcmjnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1jcns8f</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Looking for a specific thermal nail polish color</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jcns8f/looking_for_a_specific_thermal_nail_polish_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1jcufb2</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Polishes similar to Petal For A Narcissist</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jcufb2/polishes_similar_to_petal_for_a_narcissist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1jd1xmv</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>St. Patty’s day Aura</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad3x7w2eq5pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1jd6ptz</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>How can I achieve the perfect vampy nails🙏</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jd6ptz</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1jdzpsc</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Nail art !</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdzpsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1jdu57v</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>I Tried Doing a Plaid Design and Used the New Official Tartan Design for Victims of the Witch Trials</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v46duvrqtcpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1jdtk87</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>finally managed to sculpt a decent 3d flower :)!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdtk87</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1jdrvl9</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>I like doing weird things on nails sometimes 👩‍🏭💅</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdrvl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1jdqou1</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Soap nails trend. I made myself laugh which is what counts</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8f11gig0cpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1jdqhuc</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Shiny mix and match</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8t03mauybpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1jdpfje</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>How long do you think I needed for them?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uin5cfmqbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1jdoaww</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Springtime press ons 💕🌷✨</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdoaww</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1jdo6ep</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Fruit, florals, or animal?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6aztd084hbpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1jdn5no</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>What product(s) is used for stamping isolated chrome art on gel?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jdn5no/what_products_is_used_for_stamping_isolated/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1jdmsab</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>For her Disney trip ✨🐭🏰</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxyr2kw27bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1jdmdx4</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Advice Needed</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgelxt674bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1jdlzt2</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Do these even look like oranges ?😟</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eewnw3pf1bpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1jdkcyh</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Had to hop on this 3d lip trend, this was soo much fun! Happy St Patrick's day!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4o1lirxspape1</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1jdjb1z</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>from last week</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdjb1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1jdj2vt</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>alien nails 👽</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qrqsgetgape1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1jdic7h</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>A few new designs I did.</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdic7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1jdhdbi</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>First time doing my nails, how did I do?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdhdbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1jdg0jm</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>My newest set of nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sefpu8w0v9pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1jdckeu</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Lucky Charms 🍀🌈🌠🎈</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdckeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1jdcfzi</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>I love freehand designs</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpmgnkza39pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1jdawtt</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>May luck find you all today 🍀</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdawtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1jd844j</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>How do you take care of your brushes?!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chdoca46r7pe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar 19 08:11:29 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_23.xlsx
+++ b/data/collected_data/2025_03_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C519"/>
+  <dimension ref="A1:C708"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9256,6 +9256,3219 @@
         </is>
       </c>
     </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1jerefg</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>For those whose workplace doesn’t “allow” fancy nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jerefg/for_those_whose_workplace_doesnt_allow_fancy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1jer0jv</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Did I do smth wrong?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jer0jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1jeqnl1</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Green and pink nails! 🌸🌱</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ngyhn2halpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1jeqiis</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>My first try at making my own gel press ons</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeqiis</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1jepere</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Handmade nails</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyjr9uz0vkpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1jep5wk</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Press on nail glue-help?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jep5wk/press_on_nail_gluehelp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1jeoxw1</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>My BIAB Nail Journey - 3 weeks of growth!</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be3zdo8kpkpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1jeowcf</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Preferred nail length &amp; shape</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jeowcf/preferred_nail_length_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1jeoe6j</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>1.5 years of progress (and quitting nail biting and picking lol, almost there lol)</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeoe6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1jeoblz</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>So funnn! :)</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmnlgtr0jkpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1jeo75j</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>What do you think? Back to my natural nails.</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21oq62y3bkpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1jeo0ug</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>4hrs later…</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeo0ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1jengs5</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Shein Press On Nails $4</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgm20qrlakpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1jende0</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>All white, medium length,square, acrylic🤍</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jende0</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1jen3yv</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Can somebody tell me what did I do wrong?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jen3yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1jen3od</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Cow nailsss</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnoi2cj17kpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1jen07j</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>I'm IN LOVE with my nails ❤️🌈</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p10110146kpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1jemt7d</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My graduation nails 😍</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/je8jhrx84kpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1jemr7h</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Spring time</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrd8uxrq3kpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1jemr0h</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Cat eye for the win 😍</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a7rt8ulo3kpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1jemmys</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Leopard nails!</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsz12cam2kpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1jemj4z</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Spider-Man nails!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4f8f74vl1kpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1jem93o</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>New nails, sun, and thrift day!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jem93o</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1jem8wp</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>These have been on for almost 3 months.... what gel they using in Japan and where can I get it?!</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jem8wp/these_have_been_on_for_almost_3_months_what_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1jelkvx</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>A rainbow set for my cake day :)</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n95vworzsjpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1jelevj</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>They look so real! I'm amazed...</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jelevj</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1jekw48</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>My sister's nails Made by @nailar.sofi.bb</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jekw48</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1jekcz7</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>My artist @v.rnish is the coolest</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bz2sbhbijpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1jek3e6</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Queen shit 💅 ❤️ 😍</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psvwy8l2gjpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1jejkwj</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>💙🦋🧢🐳🔵</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ic2501tbjpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1jeit32</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Are these bad… what do I do</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7d5ue8bl5jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1jejbvq</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>I would like to know your opinion on acrylic nails for the toes. Do you recommend them? I've heard that they're not very good. Pic By:nailsbylolu</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnjan03s9jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1jejazz</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Love this new set</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc16tegl9jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1jeiwqt</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Got bored and… acrylic paint+clear top coat 😅😅</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr991gde6jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1jeiwhw</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Final Korean Manicure before I leave the country 🎀</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyxpcydc6jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1jeitth</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Mexican tile + lemons set</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeitth</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1jeibbf</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>My self done nails for St Paddy’s :)</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeibbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1jehylp</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sabwwjaxyipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1jehiwu</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Beautiful Design🖤🩷</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dl8y7ujvipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1jehd22</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>My best set, yet.</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lgbggqauipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1jeh770</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>press on nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jeh770/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1jeh4ab</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Shamrock and roll ☘️</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zw5f4tvfsipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1jegwbp</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>ik theyre not the best because im a beginner but current set!</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jegwbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1jegrze</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Never posted here before….</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trr48j6spipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1jeg95c</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>japan ready nails!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pntorisrlipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1jeg86r</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Green on black is my whole aesthetic, but extra happy with how perfect these came out!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeg86r</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1jefucb</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>How do we like the goo nails?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wnlz44qiipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1jefsk2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Made my very first set of press ons!</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jefsk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1jefrpy</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Birthday Nails I did on myself 💅🏻</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jefrpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1jefb7g</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Acrylics for the first time</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5emefbveipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1jef9sh</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Unhappy with the way these turned out. Is it wrong to go back and ask that they fix them?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jef9sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1jeeze8</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>My nails for rolling loud this past weekend</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dv7cpp3hcipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1jeepqt</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>First time gel x nails. Are they good?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeepqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1jeejly</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Strawberry nails!🍓✨</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smee9u5c9ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1jeea80</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Bojack set 🖤 line work could be better but I’m proud of these 🥹</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjvlx91i7ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1jee33p</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Proud of these ones</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfn3h9b26ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1jedumd</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Should I do a new set or keep these?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dmcv71074ipe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1jedr31</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Does Beautometry ever Restock their Sold out Polishes?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jedr31/does_beautometry_ever_restock_their_sold_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1jedp3m</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Northeast Louisiana</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jedp3m/northeast_louisiana/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1jedo2v</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Does this shape suit me?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w697myez2ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1jedmaj</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Organic green</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jedmaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1jedljp</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>5 Minute Mani</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnlpbesg2ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1jedica</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Roses &amp; lace French by my nail tech!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jedica</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1jed9si</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>What should I do?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jed9si</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1jed96z</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Simple but cute!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcv17lq20ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1jed511</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Clear press ons</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jed511/clear_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1jec4cd</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Anyone else have issues with DND Gel customer service?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jec4cd/anyone_else_have_issues_with_dnd_gel_customer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1jebow2</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>An evolution…</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jebow2</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1jebvc9</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Constructive criticism welcome!</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jebvc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1jebuqv</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Clean and simple.</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvv9aw00qhpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1jebjz4</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Help With Magnetic Nails</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jebjz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1jead59</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>How to prevent little bubbles from forming when applying top coat?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jead59/how_to_prevent_little_bubbles_from_forming_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1jeb7j8</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>MEGA pink sparkle gemstone nails!!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeb7j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1jeazgm</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Cuticle Help</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeazgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1jeasyp</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Can I get my bitten nails done?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jeasyp/can_i_get_my_bitten_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1jeadzt</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Do I need top coat for a soak off gel nail polish?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jeadzt/do_i_need_top_coat_for_a_soak_off_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1jea51a</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Do I use the Orly Rubberized Base Coat for gel polish or regular polish?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jea51a/do_i_use_the_orly_rubberized_base_coat_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1je9zq8</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>I got my pedicure done today, normally I choose french. Today I wanted something different.</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltr23thpchpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1je9pl7</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Frustrated</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1je9pl7/frustrated/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1je9gqg</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Im proud🫶🏽☕️</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5qxqnau8hpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1je973h</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>How to enhance my natural nails without thinning or ruining them?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/igisjjeu6hpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1je96qz</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Remove press ons without damaging nails</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1je96qz/remove_press_ons_without_damaging_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1je7juu</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Weird shape?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je7juu</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1je7uem</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Love my nails!! $4 well spent</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5spfa2vwgpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1je8cue</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Some nice clean pearly shorties 💛</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p53ehwul0hpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1je64z4</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Press on</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1je64z4/press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1je5p02</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Nail art!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je5p02</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1je2m9t</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>I did Toadstool Nails at home</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byukr04zmfpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1je895c</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>It is so reflective!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp7ihxuxzgpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1je7y3q</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Finally starting to get the hang of blooming gel!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihe8vjtmxgpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1je7sog</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>St paddys nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je7sog</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1je7r68</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>New to nails, don’t know what to get on natural nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ytdxzm5wgpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1je495n</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Men with nails like this</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy26949q3gpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1je1t9l</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>short extensions pop off but long ones hold???</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1je1t9l/short_extensions_pop_off_but_long_ones_hold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1je73jy</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Green and springy🌱</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0ayp8e4rgpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1je6vqg</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Finally went extra with my nails :)</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5r6oyqgpgpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1je6p68</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vkmdum1ogpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1je6jiz</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Any stright men who paint their nails? Colours?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1je6jiz/any_stright_men_who_paint_their_nails_colours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1je6edo</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Red pearls</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je6edo</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1je6cnx</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>What to do to help damaged nail as it grows out</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je6cnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1jeqp2e</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Gold and brown always reminds me of old money</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeqp2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1jeqof3</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>New Clionadh polishes</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jeqof3/new_clionadh_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1jeptf1</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics “psilocybin”</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeptf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1jeplf3</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>In the middle of swatching hell</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeplf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1jepf7t</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Voting reminder - Indie Polish Awards Voting Ends Sunday</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://forms.gle/eELfwtfVVhmn19y3A</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1jep5pq</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Dupe for Ethereal Chihiro</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jep5pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1jeoiqe</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - ✨Warped Expression✨</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeoiqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1jeoi5g</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Late but St. Patrick’s Day nails!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeoi5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1jeo2u8</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Pink to Purple Skittle</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeo2u8</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1jenmys</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Emily de Molly’s Orea absolutely destroyed by bowling</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jenmys</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1jenexb</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>First time trying something like this ! I love it !</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cu1s8kf3akpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1jen8lr</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Looking for a replacement polish - any ideas?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jen8lr/looking_for_a_replacement_polish_any_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1jemmtt</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>help me find this color!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jemmtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1jekfql</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Celebrating the new Hunger Games release with my Capitol Colors collection</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jekfql</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1jek582</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Organized my colors!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jek582</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1jejcek</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Beginner collection: I think I have a type (I need to branch out)</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6izxa4x9jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1jej595</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Practice makes… well, not quite perfect</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jej595</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1jeiyo3</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>help me decide if i love or hate this polish !</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeiyo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1jeirak</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>PSA: Indigo Bananas full size paddle appears to fit ILNP</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1uu63d15jpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1jei7sc</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Confessions of a nail polish junkie</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jei7sc/confessions_of_a_nail_polish_junkie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1jei24w</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Layering experiment</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jei24w</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1jehnmz</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>natural color polish recs</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp64ftvjwipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1jehlt5</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>After the Rain 🌧</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vtug0u5wipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1jehjsg</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>High vis nail polish, OSHA compliant (not really), workplace safety core.</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jehjsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1jehjf8</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>High vis nail polish, OSHA compliant (not really), workplace safety core.</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jehjf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1jehhac</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>My goblins are OBSESSED with my nail file</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syq0kwh6vipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1jehb60</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>ILNP - Bottoms Up + MPR</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uiqqngrvtipe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1jeha0f</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>first ILNP order</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1varh5mmtipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1jeh3e1</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>ILNP Venom velvetised</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/garrxxz8sipe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1jegsvq</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>omg…</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jegsvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1jegjju</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Gold/glowy skittle for spring!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k7mznhynipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1jegbq5</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>All the colors</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jegbq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1jeg2t9</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>3 months in and my nails are absolutely destroyed.</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da1lcdchkipe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1jedpoz</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Does Beautometry ever Restock their Sold Out Polishes?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jedpoz/does_beautometry_ever_restock_their_sold_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1jefvb7</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Dupes &amp; Comparison Megathread</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jefvb7/dupes_comparison_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1jefmxb</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Sassy sauce: shamrock and roll ☘️</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvkpytc8hipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1jefblw</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jefblw</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1jef1xy</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>PFD’s Lush is glowing in low light</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jef1xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1jedy77</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>I’m gonna cry when the topper runs out</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jedy77</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1jedeww</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Starrily - Atomic Clock</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/reb128g51ipe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1jec7lp</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Anyone else have issues with DND Gel customer service?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jec7lp/anyone_else_have_issues_with_dnd_gel_customer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1jebel9</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Organized to the max</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ill1bwbqmhpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1jeb6oz</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>6 months of nail care changed my nails a LOT</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeb6oz</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1jeb2c8</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Why do certain polishes get discontinued?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jeb2c8/why_do_certain_polishes_get_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1jeb239</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Frost On Leaves</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeb239</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1jeazh2</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Matcha latte nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeazh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1jeati1</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Fairy Dream</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el3m06qkihpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1jea7a6</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>What are the indie brands with the biggest catalogs?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jea7a6/what_are_the_indie_brands_with_the_biggest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1je9tc2</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>March Manis so far!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je9tc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1je9rc6</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>My first gradient attempt! Holo Taco Sweet Tooth + Pinky Swear. It’s subtle but I like it! (I dulled the Sweet Tooth down with brown and white to better match my skin tone).</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je9rc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1je9pw8</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Sunken Treasure</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9yyg4oqahpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1je8gcc</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Dupe master list</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1je8gcc/dupe_master_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1je5s6w</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>💛🩷Creamsicle Watermarble🧡💛</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je5s6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1je55ml</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>A month or so of manicures</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je55ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1jdf1p1</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>I feel like a fairy✨</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/igbuft9zn9pe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1jdi758</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>St pats</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdi758</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1jdm8aa</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Cremes for nail art. Beginner help.</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jdm8aa/cremes_for_nail_art_beginner_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1je4twq</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Jazzing up old cremes with chrome powder</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je4twq</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1je4byn</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Layering to get the “perfect” color</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1je4byn/layering_to_get_the_perfect_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1je4819</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Photos don't do this one justice!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l64r4vmf3gpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1je3ter</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>ISO true Tibberz-base-purple dupe</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jflta8ipyfpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1je2q29</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Your fav Emily de Molly shades?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1je2q29/your_fav_emily_de_molly_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1je2nhz</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>3 Colour Skittle</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jF27z1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1je1tl3</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>St Patrick's Day</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57v575qvdfpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1je1p01</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Looking for picture of hand with finger tattoos (help?)</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1je1p01/looking_for_picture_of_hand_with_finger_tattoos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1je1h9w</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Help please! Fancy gloss thermal topcoats</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1je1h9w/help_please_fancy_gloss_thermal_topcoats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1je0gai</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>ILNP essentials?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1je0gai/ilnp_essentials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1jerfv0</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Silver Green/purple metallic</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jerfv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1jepdkx</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Any harry potter fans?</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jepdkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1jeohtx</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Snorlax Nails</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4abhsqtkkpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1jelm1c</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Rainbow Birthday set!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx9oojkatjpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1jel076</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Help! My Cat eye isn’t cat eyeing!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jel076/help_my_cat_eye_isnt_cat_eyeing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1jek8ph</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>nails from vday❤️</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jek8ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1jeihto</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Making nail sets to sell for the first time (explained in the description)</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeihto</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1jei2sx</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Meh.</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8psr6oiuzipe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1jehp02</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Late St. Patrick's Nails Post</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jehp02</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1jegku1</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>How do I do this?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/8Esmg15pei4?si=ul99Zec8C-1NtA8X</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1jegjw9</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Gems/ Charms</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jegjw9/gems_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1jeeydw</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Green aura and silver accents to celebrate spring!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjcc1tfacipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1jee8tm</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Bojack🖤 I know there’s a lot to improve on but I’m proud of these 🥹</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dr6tdm77ipe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1jedp8n</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Organic green</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jedp8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1jdf97z</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Made by me, two different but similar styles, I think they are so beautiful!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jdf97z</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1je3cgg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Cute Red Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kh9we6vufpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1je37a0</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Nail art by Poetiknails</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je37a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1je2t21</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Birthday nails ready 💅🐆 subtle, classy, and a little wild 🤭</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je2t21</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1je26v1</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>I always picked red nails. Today, I wanted something different. I did them myself—I know it’s not professional, but I’m not a professional. 😀 I used pearl powder on my nails to make them shine. What do you think of my red and pearl nails?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1je26v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1je1q9a</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Experimenting with chrome 💅🏼</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxj5zegpcfpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1je0nt8</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>First spring set of the year</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqvkxiklyepe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1jczxnl</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Advice Requested</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jczxnl/advice_requested/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar 20 08:11:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_23.xlsx
+++ b/data/collected_data/2025_03_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C708"/>
+  <dimension ref="A1:C906"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12469,6 +12469,3372 @@
         </is>
       </c>
     </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1jfjin7</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Engagement shoot nails 😍💍</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpqkqfhisspe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1jfiyjb</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>how to get dried glue off of natural nails (i’m allergic! 😭)</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfiyjb/how_to_get_dried_glue_off_of_natural_nails_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1jfixb3</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>did my moms nails with gel polish , how did i do ?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muj0yvxckspe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1jfgcht</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Spring Nails!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfgcht</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1jfiklq</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Progress!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfiklq</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1jfi2w1</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>New nail set I did for myself tonight! What do you think?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfi2w1</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1jfi065</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Finding Nail Techs</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfi065/finding_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1jffd1c</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>What is this?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jffd1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1jfh1yl</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>👉👈</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b7syth1xrpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1jfh1c2</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Purple cateye ft. Sleepy puppy</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfh1c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1jfguy3</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Need new top coat!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfguy3/need_new_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1jfgtm0</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfgtm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1jfgpbe</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Love a classic red</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5t3j306trpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1jfgfrq</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Holographic pink</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfgfrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1jfgbkj</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Beginner gel x</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfgbkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1jfg9z0</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>My last nail set…$40. What nail shape should I consider?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfg9z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1jfg53t</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>first post! super new to nail art trying to get better everyday &lt;3</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hymbl2o9nrpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1jffvtd</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Baby pink with rainbow cat eye 🫶 new to this!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jffvtd</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1jfftkv</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>infrared nails!!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfftkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1jfftaq</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Fresh gel</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfftaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1jffmpe</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Lamp recommendations</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jffmpe/lamp_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1jffkcr</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>These are my natural nails, but I feel like my cuticles don't look very healthy</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8bt98jlhrpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1jff7s5</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>First attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72f6mhf7erpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1jff2c8</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Was in the mood for some sparkle</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/418mp9rqcrpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1jfem7d</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>First ever manicure that's not a set of HEB press-ons</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfem7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1jfdkg8</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>does anyone know what this design is called? source is @heygreatnails on youtube</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j749fe34zqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1jfe5cl</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Non uv base coat with semi solid glue</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfe5cl/non_uv_base_coat_with_semi_solid_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1jfe059</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Delicate light pink cat eye 💖</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykyp9z1z2rpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1jfdh6l</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Loving this Blue</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nml8c9bbyqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1jfdbsn</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Am I being obsessive or are these French tips different enough to request a redo?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmbe2vcwwqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1jfbuqc</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Loving my nails 💅🏾</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfbuqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1jfd3i8</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Did my own gel nails, are they fat?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfd3i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1jfcvj8</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>my 1st attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfcvj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1jfcupx</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccxiy5xusqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1jfbd0m</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>help! hype me up to ask for a refund!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfbd0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1jfbjcx</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>absolutely love this set. and my nail tech only charged me $45 for them!!?!?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfbjcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1jfbif9</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Purple spring nails with stickers.</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zb3o2ybhqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1jfba58</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Not bad for under $10</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfba58</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1jfawnf</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Pink rainbow chrome nails 🩷🌈💅</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq0ppvfccqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1jfavb0</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>First time doing acrylic</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfavb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1jfakl1</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Friends keep saying they look like nips, but I love them 😭 thoughts?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5bvjj0o9qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1jfaakj</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>So satisfying when you walk out with exactly what you wanted ☺️</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1hwjcyg7qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1jf9zfg</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Nail Techs: Let’s Talk About the Industry’s Biggest Gaps in Health &amp; Safety 💨</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf9zfg/nail_techs_lets_talk_about_the_industrys_biggest/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1jf9iru</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>what a chop shop done to my nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xspiixxe1qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1jfa1qm</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I've been wanting to switch from shellac to biogel for ages but I'm really scared... What are the risks?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfa1qm/ive_been_wanting_to_switch_from_shellac_to_biogel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1jf9xy4</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Fresh set, how did I do?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guher3cm4qpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1jf9rt4</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>finished my first set since letting my nails conpletely regrow. went for impressionist flower patch</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fv62sple3qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1jf9kug</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Breakfast nails!! This set took so long!!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipkf510v1qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1jf9iym</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Springtime plaid</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8neg6zhg1qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1jf9f12</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Sparkles and Holo for Spring!! ✨</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf9f12</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1jf9eb8</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Loving my first set using DND products</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf9eb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1jf92bo</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Primera publicación, aún sigo practicando! Algún consejo para mejorar la técnica? Se me sigue dificultando el sellado en cutícula</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwxn6yaxxppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1jf8w9c</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Only two coats, it’s so pretty!!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5ugjfwtjwppe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1jf8ns6</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>This Glitter Pink!!! 😍</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf8ns6</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1jf8u93</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>For the people who wanted to recreate my last one for short nails</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9hgtkf5wppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1jf8q8d</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Some of my favorites</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf8q8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1jf8mbo</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Cute Panda Nails 🐼</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94owfsgfuppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1jf8fwi</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Thoughts on these French tips?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf8fwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1jf84dm</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Been getting lots of compliments on this colour, what does everyone else think?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h92lleqmqppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1jf75e9</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Body glitter on nails?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf75e9/body_glitter_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1jf81sh</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I painted my moms nails today. Was going for a marbled look</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dc5jpk4qppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1jf7w7r</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>ASP Nail Strengthener Gel Kit</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvxax8gyoppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1jf7sxw</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Does the nail salon do refills on gel x?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf7sxw/does_the_nail_salon_do_refills_on_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1jf7fnm</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My nail tech did that cat eye affect on me for the first time! I’m obsessed! 💓 what designs do you guys get with this affect?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf7fnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1jf7e9z</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>First post! What Do We Think of the Nails I Got Today?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf7e9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1jf76uj</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>First post , what you charge for these? New and experienced nail techs pls answer</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s72nttqjppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1jf763a</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>More neutral nail!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtlgqt5ljppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1jf57j0</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Help a motha out</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf57j0/help_a_motha_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1jf6gm6</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Strawberry set🍓</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf6gm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1jf6axs</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>spring nails!! baby blue coffins 💙🦋</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf6axs</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1jf668b</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Spring nails from last year 🌸💐diy</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf668b</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1jf5mox</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Dreamy nails ✨</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlmp5xdb8ppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1jf5fnh</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>How bad is it?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf5fnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1jf5b2o</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>For the DIY Gel nail girlies….</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf5b2o/for_the_diy_gel_nail_girlies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1jf59yf</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Soot sprite nails! DIY and so proud of the result.</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf59yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1jf51ki</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>My nail tech is incredibly talented! They transformed my nails with this amazing design. Feeling fabulous!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf51ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1jf50p3</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Drawing stars is hard omg</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf50p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1jf4rfz</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Any ideas on how to help this nail heal better?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dc4yer02ppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1jf4u2z</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Minimal pink</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbw79dtd2ppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1jf4qks</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>some sets i’ve done</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf4qks</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1jf4lja</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Has anyone’s nails been broken because it hit the artificial nail?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf4lja/has_anyones_nails_been_broken_because_it_hit_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1jf4ixc</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Recommendations for first time press-on wearer?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf4ixc/recommendations_for_first_time_presson_wearer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1jf4gv8</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>I was just gonna do one accent nail lol</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf4gv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1jf434k</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>New set :)</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf434k</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1jf3zy7</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>What type of nail care you need when using fake nail?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf3zy7/what_type_of_nail_care_you_need_when_using_fake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1jf3ewh</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>What do you think of them?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53qyw0p2sope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1jf2wxn</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Feeling like myself again 🥰</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmla442hoope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1jf2rxf</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>First post! Do we fw these?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx4mvmognope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1jf2pnz</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Is this faint line under the white part of nails normal?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf2pnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1jf1xf0</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Help! Wide nail beds!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqexlxz6hope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1jezmtb</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Why does my nail polish do this??</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jezmtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1jf1m4g</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Help Oil staining nails</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf1m4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1jf0jf2</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>What's the best hand lotion?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jf0jf2/whats_the_best_hand_lotion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1jez706</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>people who work in trades, how do you keep your nail polish nice?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jez706/people_who_work_in_trades_how_do_you_keep_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1jeytl1</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>My March set</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeytl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1jewtc1</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Chrome around edges</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jewtc1/chrome_around_edges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1jeql1u</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>How do I Prevent This Flaking on my Nails?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5diqjdpk9lpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1jez4pw</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Can I use OPI nail polish on soft gel and top it off with a gel top coat?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jez4pw/can_i_use_opi_nail_polish_on_soft_gel_and_top_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1jeyws8</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Classic white!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/za2iz7pjunpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1jeywi3</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Went to get my nails done after 5 years of doing them myself</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeywi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1jfjcpw</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Barry M blue margarita. 2 coats freshly painted</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfjcpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1jfj25v</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>My Severance Manicure👩‍💼💅</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfiz5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1jfisyf</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>This immediately became one of my favourites. Bee's Knees in I just want to spank it out of him.</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfisyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1jfhl8t</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>dnd lacquer in orange smoothie</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dns2yuu83spe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1jfhhto</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Betelgeuse</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7w0x3m42spe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1jfh6dv</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Can anyone tell what my favorite color is?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okgkr0ngyrpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1jfgnst</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Culprit’s Charm 🍬</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfgnst</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1jfggcq</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Pretty proud of this gradient</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfggcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1jfgeag</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Essie Cut It Out - OPI Significant Other Color</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfgeag</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1jffbj7</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Starrily’s Diamond Rain is gorgeous</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jffbj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1jff5ba</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>What polishes are currently on your wishlist?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jff5ba/what_polishes_are_currently_on_your_wishlist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1jff355</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Color Club Help - I think it's mislabeled.</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jff355</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1jfew0c</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>joining the painted cabochon club 💎</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfew0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1jfem1r</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Recs for a thermal that turns bright/lime green when warm? (Hulk-ish)</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfem1r/recs_for_a_thermal_that_turns_brightlime_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1jfehji</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Praise Kier, my outie's manicure is mysterious and important. Thanks reddit!</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq7fru3c7rpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1jfeeqj</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Lurid Haul WITH PROTOTYPE SPOILERS</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfedyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1jfe8vz</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Orly said stfu about Avacado Green already 😭</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zu0suz55rpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1jfe8p9</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Press-ons for tiny baby nails??</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfe8p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1jfccoe</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>topcoat all of a sudden causing shrinkage ?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfccoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1jfc2f5</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Clionadh-you’ve done it again!</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfc2f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1jfc0hy</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>I just had to try this combo 💚🩵</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8af6e7fklqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1jfby4f</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>BKL and nail shape…</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfby4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1jfbvf7</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Whimsical Nail Polish by Pam- Peanut Butter and Jelly</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfbvf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1jfbhpd</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>New account, more Base Coat Battle!!!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfbhpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1jfbe37</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Need Help Finding A Dupe</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfo6typbgqpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1jfbcgn</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>The way i store my magnets. I thought this might be a good idea to share</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81eobkdyfqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1jfaxvk</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Boot scootin’ BOO-gie</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk55grzmcqpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1jfako2</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Can’t decide between Cirque’s or Mooncat’s base coats</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfako2/cant_decide_between_cirques_or_mooncats_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1jfa06d</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Are HHC and PPU’s shipping windows similar?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfa06d/are_hhc_and_ppus_shipping_windows_similar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1jf9i7e</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Sparkles and Holo for Spring! ✨</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf9i7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1jf9hcp</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Springtime plaid</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0xgpkk31qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1jf8ueo</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Anyone with some serious polish knowledge?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jf8ueo/anyone_with_some_serious_polish_knowledge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1jf8slz</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Guess the Lumen polish used over Essie dark green!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hso18uasvppe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1jf8io5</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>HELLLP!?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf8io5</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1jf8i5o</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Mooncat Sagebrush</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf8i5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1jf8fmo</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>What’s your favourite type of nail polish bottle/handle?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkbjy050tppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1jf8dc9</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Any Canadian alternatives to Essie</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jf8dc9/any_canadian_alternatives_to_essie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1jf7i5g</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Unexpected combo?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf7i5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1jf6sim</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Such an interesting color shift!</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e7uqtvdpgppe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1jf6sce</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Thank You for Loving me on natural nails 🕯️🩶</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf6sce</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1jf6rln</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Interview nails! 💅🏻</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npv3gytigppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1jf6oko</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Thermal polish texture?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf6oko</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1jf6nv1</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>So shifty</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf6nv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1jf5vwb</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Got a huge lot of free nail polish from a friend!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf5vwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1jf5so9</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okuafppj9ppe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1jf5mx6</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Simple look but just feeling happy I started doing my nails again and had to share</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf5mx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1jf5452</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf5452</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1jf4bvd</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>So Franken Cute</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf4bvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1jf3z9q</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>The sun made me nails look prettier</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fcs9e37wope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1jf3nap</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>spring break vibe</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf3nap</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1jf3jq5</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>St. Patrick’s skittle</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39o8iol0tope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1jf3gyj</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Help me choose a polish for this outfit</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jf3gyj/help_me_choose_a_polish_for_this_outfit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1jf2nr6</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Okay spring snake vibes 🐍</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tilbrazemope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1jf2mur</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Brown and gold glitter frenchies</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf2mur</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1jf2k03</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>another clover appreciation post 🤩</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf2k03</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1jf2769</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Fairy Fountain🧚🏻‍♂️💙</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf2769</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1jf24ts</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Unnamed sassy sauce thermal. Does anyone recognize it?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf24ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1jf1f6c</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Two nails accidentally stained bright pink 🙃</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hd8khjidope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1jf15nl</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Help me pick a Lumon-esque color for Severance party!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsgzkeugbope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1jf0ae8</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>ILNP Aspen 💙💚</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf0ae8</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1jf029m</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>What do we think will be in PPU Rewind so far??</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mkruoma3ope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1jf025o</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Best opaque white?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jf025o/best_opaque_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1jezz1a</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>LA Colors Passion Play</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jezz1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1jezcth</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>I'm fascinated</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jezcth</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1jeyw04</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Clionadh Psilo Siblings are stunning. Photos don't do them justice.</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeyw04</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1jeyrci</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Y’all. I used to dislike glitter…</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jzxoibjatnpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1jeyjjq</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Remembered rhinestones exist!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeyjjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1jeyfs9</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>🩷❤️HAWT Hump Day Gradient🧡💛</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jeyfs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1jey0v2</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Looking for this pink colour seen online</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p54wkhcfnnpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1jex0nt</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>ILNP high roller</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w19zyjc5fnpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1jewyy2</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Jade Gemstone Nail Art 💚</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jewyy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1jewyxw</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Dart Time Lover 💚</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jewyxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1jewdne</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>I cannot even begin to explain how happy this makes me.</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jewdne</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1jewcjp</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Palette cleanser, anyone?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jewcjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1jew3or</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Is Kathleen &amp; Co the same Kathleen as Lights Lacquer?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jew3or/is_kathleen_co_the_same_kathleen_as_lights_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1jevn21</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Good nail oil?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jevn21/good_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1jevk99</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>New nail tech might have destroyed my nails 😭 (post black nails)</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jevk99</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1jeuhsn</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>LOVE reflective glitters</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6581k57qmpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1jeuape</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Keeping track of 2025.</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep3bxi2znmpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1jfjjom</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Ghibli nails! 💅 🔥</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjheridxsspe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1jfjhuj</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Surprising my friend with nails!!</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jfjhuj/surprising_my_friend_with_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1jfg971</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Fidget Spinner nail</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rx6hkt9horpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1jferpq</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Beautiful Sins by Cuticle Qween</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/liv2mbtz9rpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1jfdbd2</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Does anyone know of a place that would teach nail art basics?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jfdbd2/does_anyone_know_of_a_place_that_would_teach_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1jfcqth</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I’m a venomous keeper and I asked my nail tech Ash-lee to put my black mamba on my nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfcqth</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1jfa855</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Some sets I’ve done recently 💅🏽</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfa855</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1jfa2vl</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>For the wizard fans ✨⚡️</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63svs7zs5qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1jf9zxv</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Swipe for the inspo ✨💜</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf9zxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1jf9j48</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Sparkles and Holo for Spring! ✨</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf9j48</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1jf9ick</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Springtime plaid</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyct55jb1qpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1jf7jfj</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Coraline Nails!</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf7jfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1jf6hbl</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>New strawberry set 🍓</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf6hbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1jf2ywb</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Absolutely love this edgy silver set🖤🩶                       https://www.facebook.com/share/18TQnXNwYC/?mibextid=wwXIfr</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf2ywb</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1jf1pgl</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>They're basic, but I'm proud</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s1t4swlfope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1jf1k2n</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Un diseño de Halloween en Marzo</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf1k2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1jf1jqx</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Un diseño de Halloween en Marzo</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf1jqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1jf1d66</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Made these for my uni art expo but when i realized they were in the lesbian color and HAD to keep them</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf1d66</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1jexwwv</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Eclectic vibes all the way</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jexwwv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar 21 08:11:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_23.xlsx
+++ b/data/collected_data/2025_03_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C906"/>
+  <dimension ref="A1:C1105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15835,6 +15835,3389 @@
         </is>
       </c>
     </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1jgb3hf</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Currently a nail student, pretty happy with this set I just finished!</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgb3hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1jga3qu</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>nail healing product recommendations?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jga3qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1jga8n6</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>guys pls help. isn’t this tool supposed to say tensed? it keeps popping out and hitting my hand as i try to clip.</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rryxvjlfizpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1jga4rp</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>An asymmetrical metallic look 😍😍😍💖</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jga4rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1jga46y</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9rkw0yvgzpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1jga00g</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Natural look 👀 gel x style nails with rubber gel overlay</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mejs2wyffzpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1jg9xx4</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>My very first nail extensions</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56ouczfpezpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1jg9rt9</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Looove</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg9rt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1jg92ca</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Did my own nails today</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg92ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1jg8jqg</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>nails by @vivxue - what products for this effect?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg8jqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1jg8uch</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg8uch</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1jg8tn9</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>had to get this red cateye!</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q91r6ui1zpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1jg8c7r</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>My first time getting acrylics!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg8c7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1jg8gyr</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>I’ve been trying to “grow” my nail bed</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg8gyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1jg8e2h</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>How my nails?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgg8zr6vwype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1jg86et</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Cateye Nails</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qnd5fypmuype1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1jg7re0</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Frutti Tutti!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg7re0</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1jg85y4</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>how does your job impact your nails?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jg85y4/how_does_your_job_impact_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1jg7xam</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Matching Upper and Under</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1a686yvrrype1</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1jg7vk4</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Similar gel color recommendations?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4tzwzyirype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1jg7ujg</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Just did some press ons. Do they look good and any tips</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg7ujg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1jg7gpw</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>My favorite so far</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg7gpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1jg753v</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Did my nails first time in a while (2 months lol) How much would these cost if getting done?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swco157ckype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1jg6vyw</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Look at my nail progress over past 2 months!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg6vyw</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1jg6p5i</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>equinox vibe 🌌🌕</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19c28fu1gype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1jg6jxk</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>acrylic nail techs please help</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jg6jxk/acrylic_nail_techs_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1jg6h4i</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>what’s your favorite nail shape? i 💖 stiletto &amp; square</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg6h4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1jg6f67</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Whimsy for spring</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9yafy7ldype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1jg605g</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>My last lovey dovey set ❤️</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv2c6czp9ype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1jg5k3x</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kouywek5ype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1jg5apy</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Douyin inspired</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg5apy</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1jg5fc1</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>The way I would literally do anything for my nail tech 😩😍</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg5fc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1jg5bkv</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Burgundy w/ purple-green cat eye</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg5bkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1jg5b45</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Neutral cat eye</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so0l2uoa3ype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1jg502r</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Bob's Burgers Nails</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zg1ddspe0ype1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1jg4zpd</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Green &amp; Gold St. Paddy’s Nails</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg4zpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1jg4vqv</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Guys this shit is hard</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy268kabzxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1jg4njd</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>it's pastel season</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg4njd</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1jg4bus</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>3d nail artists, help!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jg4bus/3d_nail_artists_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1jg459n</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Rate my press ons 😝</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg459n</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1jg4599</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Silky pink with gems</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymorr70psxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1jg41t6</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i03koxvrxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1jg3z1v</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>I’m inlove with my birthday nails and had to share with someone</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg3z1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1jg3pkj</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>which shape/length should i keep my natural nails?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg3pkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1jg3osn</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Salon says I need to be able to do full sets in 45 min?!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg3osn</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1jg1h50</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>how do i apply powders?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jg1h50/how_do_i_apply_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1jg16w4</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Should I Go to a New Salon?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jg16w4/should_i_go_to_a_new_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1jg3h21</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>My latest set of press ons might be my favourite ever</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg3h21</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1jg372g</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Sailor Moon Nails</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg372g</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1jg36yb</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Deep purple</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg36yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1jg31wm</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>First time doing my own nails at home</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f4xtsecmjxpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1jg3140</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Cat eye 🐈</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg3140</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1jg2j7t</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Simple chrome 🤍</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lg7rocjdfxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1jg2csr</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Going in for a manicure, Help!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg2csr</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1jg26zk</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Bday set for my sister</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp9fiftncxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1jg23z8</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Green Freestyle</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wz1q6mczbxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1jg1xpy</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Lil mushroom ghosties</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg1xpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1jg1uuf</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>A few of my recent sets ✨</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg1uuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1jg1qiv</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Kirby nail art 🎀</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg1qiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1jg1gyy</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I feel like I have magic powers !</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg1gyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1jg1dxg</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Easter Glass</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pmcbwye6xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1jg156p</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Does anyone else have nails that stick up like this? It’s most offensive on my pinky!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg156p</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1jg133r</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Can I file custom press ons?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jg133r/can_i_file_custom_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1jg0tcu</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Blue Galaxy Nails - cat eye</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kja00mz32xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1jg0rz1</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rw3b09t1xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1jg0oj4</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Simple french and I feel anything but simple 🥰</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ddblct21xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1jg08bn</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>What color(s) should I do ?!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i8uxleoxwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1jg03jw</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>One of my pinky nail beds is huge?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg03jw</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1jfzz53</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>First time posting, matte black and dog’s paw 🐾</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1eimd3qvwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1jfztuj</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Turquoise and Tortoiseshell</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1ww2fbmuwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1jfzs1q</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>braved up and finally asked for a cute design &lt;3</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfzs1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1jfzj6l</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Too basic??</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfzj6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1jfzdd6</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>pastel chrome rainbow🌈💖</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7qj00d7rwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1jfzau5</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Opinions, please.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfzau5/opinions_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1jfz683</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I usually don't go for this shape but I think these look nice. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfz683</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1jfz0cr</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Milky white + pearl chrome</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfz0cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1jfyxi5</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>did my nails, cat eye polish, took me 8 hours 🥲</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/czmtvyyqnwpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1jfyqjp</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Naked.</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfyqjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1jfyqb6</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Do these french tips look normal?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfyqb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1jfyo98</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>St. Paddy's Day press-ons</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfyo98</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1jfyk4k</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>First Time Dip- Is this typical?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfyk4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1jfygol</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>I’m obsessed with cat eye nails</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6fojcvakkwpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1jfya5t</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Frenchhh🌸🌸</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u97vlp8jwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1jfwwzl</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u736h2y69wpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1jfwuv2</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Can I develop gel nail polish allergy if I use semi-cured nail strips?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfwuv2/can_i_develop_gel_nail_polish_allergy_if_i_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1jfxnw0</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Press on nail stands</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfxnw0/press_on_nail_stands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1jfxgrd</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Easter Nails 💅🐇 Critique Encouraged ~</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfxgrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1jfxbea</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Which nail shape?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfxbea</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1jfxaj4</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Do these french tips look normal?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfxaj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1jfwnxc</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Arcane Nails</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfwnxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1jfw1ng</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Long time lurker, first time poster👏</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfw1ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1jfulv6</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Can anyone recommend these?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfulv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1jfvwgj</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>What nail shape for my hand?</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfvwgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1jfvres</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Stained glass nails</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfvres</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1jfvqi5</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>🤍✨ New Set ✨🤍</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8fv0t9i0wpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1jfuwjh</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>My daughter finished these the other day! I love her creativity! Any tips for her?</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zliy4zuduvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1jfutdo</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>I LOVE THEM ❣️ This intense red looks great</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib2g96dstvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1jfuneh</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Ms. Pac-Man</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfuneh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1jfu9p7</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Nails smell like cat pee</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jfu9p7/nails_smell_like_cat_pee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1jftnoc</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>dirty-martini obsessed gel set</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgduiedalvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1jga73t</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>No more fried eggs for spring</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jga73t/no_more_fried_eggs_for_spring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1jg94x4</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>My wife's latest set</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg94x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1jg8uen</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>This is your PSA to buy little plastic roses and paint the backs of them</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg8uen</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1jg8l40</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>This is some 👻 boo sheet</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/broutotxyype1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1jg7901</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Opinions on BLACKHEART nail polish?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jg7901/opinions_on_blackheart_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1jg6dfk</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Happy official Spring, everyone 🌷🌧️</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg6dfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1jg5hk7</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Sassy Sauce does it again</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg5hk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1jg5gcw</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Tell me about the cheeriest, most joy-giving polish you own.</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jg5gcw/tell_me_about_the_cheeriest_most_joygiving_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1jg3vph</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Got my first Hella Handmade Creations order!</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg3vph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1jg3u4f</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Watch me glow</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6prj5cnipxpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1jg3q7r</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Shimmery grey purple velvet look.</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5jr4f55pxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1jg3gys</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Trying to find fast drying polish for young kids' nails</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jg3gys/trying_to_find_fast_drying_polish_for_young_kids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1jg34do</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Accidental combos?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg34do</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1jg2t8r</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Saw that I had eyeshadow that looks like sand, so I smashed it on my nails 🏖️</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg2t8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1jg2juh</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Polish manicure</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgbyy1zhfxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1jg1d55</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Looking for a polish similar to my mom's one</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg1d55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1jg16uy</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Anyone else miss Live Love Polish? [Throwback Thursday]</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg16uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1jg0vad</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Bliss kiss vs. plain jojoba</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpnhd59j2xpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1jg0r6f</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>What I wore in February</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg0r6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1jg0nst</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Ether Unicorn 🦄</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t19e7gxw0xpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1jg0amw</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Cirque's Vice collection release date?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jg0amw/cirques_vice_collection_release_date/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1jfzr3x</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>What It Takes🧲🩵💜💖💙</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o2n2j0tytwpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1jfz7qc</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Yo Illinois/indiana Lacqueristas!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfz7qc/yo_illinoisindiana_lacqueristas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1jfyq0f</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>PSA: If you’re looking to organize your collection, the IKEA Alex 9 drawer unit is on sale</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfyq0f/psa_if_youre_looking_to_organize_your_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1jfy20t</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>BKL Bad Manners</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfy20t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1jfy170</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>finally embracing matte</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfy170</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1jfxzl1</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Went back to shorties!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8wh8q36hwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1jfxm71</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>So Fresh and So Preen</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfxm71</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1jfwy4d</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Bermuda Triangle Dupe??</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfwy4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1jfwvjp</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Can I develop gel nail polish allergy if I use semi-cured nail strips?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfwvjp/can_i_develop_gel_nail_polish_allergy_if_i_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1jfwrf4</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>✨ Immortal manicure ✨ It has survived packing, traveling, snorkeling, boogie boarding, etc with zero chipping. 1st photo: day 11, 2nd: day 3</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfwrf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1jfw9sg</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Shoutout to BKL- Choose Life</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/954krnni4wpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1jfw40v</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>skittle of my February HHC order including my first attempt at magnetics :)</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfw40v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1jfvzda</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>What can I do about this?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfvzda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1jfvyi6</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Sally Hansen Nail Rehab is the MVP</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfvyi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1jfvtc4</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>like four different green polishes in one ✨️</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfvtc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1jfuxos</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨CLE DE PEAU</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgerqf1muvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1jfuvqj</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Garden Party 🌸</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqp1mlh8uvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1jftnps</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Spring Flakies - Card Trick</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jftnps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1jftm92</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>I'm in love!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jftm92</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1jftg9s</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Can you help me figure out a mystery gel polish brand based on a bottle description?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jftg9s/can_you_help_me_figure_out_a_mystery_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1jftb79</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Someone's going to have to physically restrain me from velvetizing every mani forever now</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lh0wqfpoivpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1jft4bw</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>First try with magnetics</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dze7ipd7hvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1jfss15</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>New Holo Taco?!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j87pau7nevpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1jfsjxx</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>First day of spring mani change</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfsjxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1jfsgea</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>1st Day of Spring Set</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfsgea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1jfs4pd</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Spring inspired: dirty melting snow piles with hopeful vibes</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfs4pd/spring_inspired_dirty_melting_snow_piles_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1jfs3a1</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Psilocybin velvetized and cat-eyed 😻</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3yfglvkf9vpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1jfs15y</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Soft spring mani 🌸</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuodcjo09vpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1jfqpnb</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Issok</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfqpnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1jfqfzb</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Mooncat Maelstrom</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfqfzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1jfqeka</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Pretty Pretty Disney Princess Nails!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfqeka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1jfqdi1</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Are these safe gel ingredients?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhwo0diyvupe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1jfqb2k</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>i love spring bc it means springy themed manis 🐸</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfqb2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1jfqayt</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Please try to enjoy each nail equally, but show preference for the index over the others because it took forever 😫</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/JUGtz5A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1jfpotm</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>🔥👁Eye of Sauron👁🔥</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfpotm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1jfpbsy</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>It's cold and snowing, but it's still the first day of Spring!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqefj2h7nupe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1jf0aw5</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Cuticula Frozen Memories</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcd10bi45ope1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1jf4135</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Still getting lifting on free edge</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf4135</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1jf9kp2</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>What a Pearl Wants (KBShimmer) Over Ivory Tower (Holo Taco)</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jf9kp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1jfbokp</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Flakie topper recommendations</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jfbokp/flakie_topper_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1jfdcuo</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Help identifying when this Revlon polish was made?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfdcuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1jfo5gl</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>These nails are whiter than my future</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi462ziscupe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1jfnxck</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>indomitable 💜</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfnxck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1jfn4t1</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Orly Harry Potter Collab</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cc484xvm2upe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1jfmhme</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Strangeberry 💕🦩🍉✨️</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfmhme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1jfkmjo</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Needed to express my free will</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c1a040e8tpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1jg8f34</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Black and gold 💛 🖤</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lre73v16xype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1jg791t</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>IG@NailsbyTim6. What y’all think ?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlep1rgdlype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1jg6u2l</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Uñas sencillas pero lindaso</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gefff7ahype1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1jg6mtc</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Pearl fever</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg6mtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1jg6c4n</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Blueberry nails</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg6c4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1jg5ww5</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>some eye practice</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg5ww5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1jg4rx0</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>First attempt at making press-ons!</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1u1zb8dyxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1jg4etq</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>3d nail artists, help!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jg4etq/3d_nail_artists_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1jg4chb</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Simple accent nails</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2twbvb5kuxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1jg4a6t</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Purple on purple</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crzsatiytxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1jg45q6</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Martini Olives anyone? 🫒</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68h874iusxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1jg44r2</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Short square frenchies</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdk8037lsxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1jg3ggy</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Hawaiian Rollercoaster Ride 🌊 🌸🐚</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2op0dfvmxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1jg213v</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Feedback on these</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt1x3z9dbxpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1jg1gcc</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>SoftGel - I'm not entirely convinced by the design😵‍💫</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2pjoo2q6xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1jg198s</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Magnetic beating heart 🖤🩶</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/787s8ome5xpe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1jg0m1y</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>beginner sets!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jg0m1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1jg0jf1</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>It’s giving 90s whimsy goth</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tiriq9c00xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1jfz27a</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>The prettiest nail medley, pure nail art. What would you add?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jll93fyxowpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1jfy22f</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>I did this at 3 AM, I want credit for not falling asleep while doing little hearts 😅</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2gfrannhwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1jfxc0o</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>The Garden 🪴</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gc374u9cwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1jfw9yl</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Which one?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfw9yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1jfw2ct</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>First time doing 3D charms</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfw2ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1jfvnou</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>What’s the Most Complimented Nail Design You’ve Ever Had?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jfvnou/whats_the_most_complimented_nail_design_youve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1jfuvxp</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Nothing better than freshly made nails</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s69men9uvpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1jfrn8v</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Coroline art</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfrn8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1jfqubn</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Set playero. Cuál te gusta más ?  🌊🏝️🌸</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfqubn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1jfp55v</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>First time making number on a nail it not as bad as i thought i would do</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfp55v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1jfp0xw</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>simple french 💅🏼🌼🤍</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nd7xm1qpkupe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1jfnhpf</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Sweet and Simple 🌸🍒✨</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzci9rxk6upe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1jfmpl5</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Hyperfem strawberry nail set</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfmpl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1jflmgs</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Have to say...</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zaj2128gltpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar 22 08:09:59 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_23.xlsx
+++ b/data/collected_data/2025_03_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1105"/>
+  <dimension ref="A1:C1297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19218,6 +19218,3270 @@
         </is>
       </c>
     </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1jh31hr</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>March nails</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rmruwqg07qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1jh2vy5</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Aqua blue with white flowers</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxz620wcy6qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1jh2r8x</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Structured manicure question</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jh2r8x/structured_manicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1jh2ed5</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Which is your favorite?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh2ed5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1jh260m</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>how to get really defined cat eye</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgpusntto6qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1jh22ag</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>grown out nails</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb7np7ojn6qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1jh17kb</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Taking a break from Gelx</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh17kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1jh14st</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Should there be a gap between gel x and nail?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh14st</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1jh107j</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Summer vibes ☀️</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0reapi0wa6qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1jh0zij</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Birthday nails! (Late post my bday was 03/14</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1cf1mqkoa6qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1jh0rfq</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Give me your opinion ☺️</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh0rfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1jh0o59</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Newest set of pressies 💅</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh0o59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1jh0efx</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>nails help! gel keeps chipping 3 hrs after manicure</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jh0efx/nails_help_gel_keeps_chipping_3_hrs_after_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1jh065t</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Some new sets I made :)</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh065t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1jh03cp</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Birthday nails✨</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmlwt33z06qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1jh01km</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Manifesting summer cause I'm sick of the cold</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh01km</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1jgz1xw</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Trying to get into doing nails</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgz1xw/trying_to_get_into_doing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1jgyoip</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Press ons?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgyoip/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1jgyils</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>anyone else have a very hands on job that results in you never being able to keep ur long natural nails? 💔</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgyils</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1jgyfej</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Are these considered long for acrylics?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m92d4uykk5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1jgy62x</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Can I put press ons over Sally Hansen Hard as Nails?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgy62x/can_i_put_press_ons_over_sally_hansen_hard_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1jgy5zn</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Asked for coffin, I think I got more square. 😭</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x10w3592i5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1jgy3to</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Pastel spring Easter nails</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgy3to</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1jgy3fz</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>New Set 💟</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dvvy6xdh5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1jgy2xa</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>What vibes do my left and right hand give ?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgy2xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1jgxw6q</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>HK/ sweets and treats nails</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgxw6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1jgx9md</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Miffy inspired nails</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgx9md</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1jgt8kb</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>My Disney nails suck!! What could I have done differently?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgt8kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1jgxpxd</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>I did my best haha</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aky6iu0xd5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1jgxlia</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Ethereal Vibes</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgxlia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1jgxhf0</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Fiancé picked my set again</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kel51oiqb5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1jgx5a3</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>How bad is this</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgx5a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1jgx549</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>How bad is this</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgx549</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1jgx4zk</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Hello! Do you like my new design?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iavl5opk85qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1jgx20j</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Is there such a thing as DIY blooming nails?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgx20j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1jgwzjz</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>It's spring!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfrql9o675qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1jgws8e</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>New Press On Design I tried today</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgws8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1jgws1v</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>New Press On Design I tried today</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgws1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1jgvqiu</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>DINO Aqua Peach- how to improve?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ms7zzrh2w4qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1jgwp7i</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Simple and clean are my favorite [Luminary Gel]</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58tqekrl45qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1jgwawe</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>I usually get stiletto, but fancied a change. What do ya think?</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgwawe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1jgw7st</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>I got my first full set today</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgw7st</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1jgw0pb</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>I'm loving 💖💖the ruber, who prefers ruber or other</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijesmaxjy4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1jgvvbr</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Nail tips I turned into press-ons</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yllh9w89x4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1jgtb14</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>First time.</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgtb14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1jgulzw</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>How to stop trimming cuticles?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgulzw/how_to_stop_trimming_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1jgvixi</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Miffy x Scrapbook-y Nails!🍒</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgvixi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1jgtae1</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Am I now allergic to gels? I get blisters along my cuticles. ☹️</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgtae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1jguz1w</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Not me trying to keep track of all my manis instead of sleeping…😅</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyjnkqmnp4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1jguc5g</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Press-on recs for wide nails</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jguc5g/presson_recs_for_wide_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1jgu9br</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Spring Nails! ✨</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgu9br</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1jgu94n</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>For those of you saying my bad mani looks like teeth…</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgpd1acqj4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1jgtz3r</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Can I go over nails that are already done and top coated?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgtz3r/can_i_go_over_nails_that_are_already_done_and_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1jgtonc</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>my fake nails dont even stay on for one full day !</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgtonc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1jgtocq</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Are we sick of green yet?</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgtocq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1jgsj6k</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Longevity of press ons with polish glue underneath??</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgsj6k/longevity_of_press_ons_with_polish_glue_underneath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1jgrhfk</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Mail help needed</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bztz8qtkx3qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1jgtao6</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Feel put Together</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5r7l7mxxb4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1jgta36</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Should I ask for my money back?</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgta36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1jgsznq</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Spring Nails- Powder Pink 242 DND</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgsznq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1jgswgf</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Nail polish color match??</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb4luy2s84qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1jgsj4k</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>hi all! i'm looking for suggestions!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgsj4k/hi_all_im_looking_for_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1jgs9lv</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>what colour nails would give bisexual energy??</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgs9lv/what_colour_nails_would_give_bisexual_energy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1jgs6z6</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Struggle with nail shape</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgs6z6/struggle_with_nail_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1jgryiw</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>First set of press ons coming out my small business!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwuc6hfa14qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1jgrlgm</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Gelx worth $110?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgrlgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1jgqrh2</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>1 Month of Nail Care!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgqrh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1jgq7x5</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Why is my nail like this?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgq7x5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1jgqh8t</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Nail bed broke under acrylic . Help!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxjncuoxp3qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1jgq86y</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>kept it simple</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgq86y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1jgq0v1</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>press on tips!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgq0v1/press_on_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1jgpxog</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>"Swearing doesn't make you cool" - Omni-Invincible Fanart</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgpxog</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1jgpsvw</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Any tips welcome. This is very clean for me and only my second attempt.</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgpsvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1jgpgap</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>March Nails 🍀</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51bs99cai3qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1jgp6s2</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Spring 💐</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgp6s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1jgp2c4</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>White and silver</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxpusxnbf3qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1jgown6</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>In love with cateye</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/idwhoi44e3qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1jgoven</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Tips for doing gel</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgoven/tips_for_doing_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1jgoupo</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Easter 🐣 Nails 💅</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwvsp12qd3qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1jgolvr</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Overfiled nails</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgolvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1jgo6jn</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>What kind of manicure should I get when I’m trying to grow my natural nails?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgo6jn/what_kind_of_manicure_should_i_get_when_im_trying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1jgok4s</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Another claw shaped nail, another good day</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgok4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1jgojkz</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Nails I did on myself for a vacation</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgojkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1jgohqy</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Nails of the day</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgohqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1jgoabk</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Apple core</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgoabk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1jgo5ke</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Short Stiletto Hybrid Polygel nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgo5ke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1jgo5hv</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Recommendations</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s6bq9yi83qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1jgo43e</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>I literally trust my new nail tech with my life</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boans54883qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1jgo3jp</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>I’m severely obsessed🤎🌺</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfm2gj5483qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1jgnu3f</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>My Nail Lady has a special place in my heart 🤭❤️</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7cygkq563qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1jgnnyl</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Hi everyone I’m visiting my LDR and she is upset she couldnt do her nails before coming to me - what can I pick up at target as someone that knows nothing about nails?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgnnyl/hi_everyone_im_visiting_my_ldr_and_she_is_upset/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1jgnjh3</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>I just got these ones and I’m so obsessed 😭 my new tech is amazing</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zarid0xw33qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1jgn6xk</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Just got into press ons and I'm in love</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgn6xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1jgmaco</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Help! How do I prevent acrylic from bulking at sides?!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgmaco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1jgmfwy</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Toddler sized hands</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgmfwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1jgcujo</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Press On Nails &amp; Glue?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/taktdoyrh0qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1jgcxt4</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Gel nails lifting and breaking</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0s56k8h0j0qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1jgkxhh</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Working on my first set of nails 💅</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b88egj8qk2qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1jga8j7</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>onycholysis</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zkcd3oaizpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1jgl61v</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Do/when should I get a fill?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgl61v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1jh2sd4</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Experience with nail stickers? These ones are from Deco Beauty</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h8gxcd0x6qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1jh2mrr</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>I used Orly thinner in a couple of shimmer polishes before knowing it was a bad idea. Have I ruined them permanently?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jh2mrr/i_used_orly_thinner_in_a_couple_of_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1jh1o4g</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Thermal Shenanigans</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw75zuloi6qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1jh1n6d</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>I just want to say THANK YOU!</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh1n6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1jh1llx</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>I just want to say THANK YOU!</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh1llx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1jh0ydw</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>The shimmer topper possibilities are ENDLESS</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh0ydw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1jh0iug</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Dawn of Empire - Mooncat</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh0iug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1jh09qb</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>LynB Amate (thermal) vs. HT Going Solo</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh09qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1jh01d6</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>can anyone tell me what i’m doing wrong? top coat causes lines/ridges to appear</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0riw0we06qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1jgzli0</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Did I Screw Up with Modified "French Nails"?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgzli0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1jgze3n</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>New to the hobby, these are my second set!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n257b850u5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1jgyw74</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Dissapointing Hyped Polishes</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgyw74/dissapointing_hyped_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1jgxuth</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>QDTC, apply when polish is wet or dry?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgxuth/qdtc_apply_when_polish_is_wet_or_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1jgxr2z</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Dupe recommendation?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgxr2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1jgx9wa</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Referral Code</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgx9wa/sassy_sauce_referral_code/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1jgwvrp</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>How do you swatch magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgwvrp/how_do_you_swatch_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1jgw0le</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>I love a good LA Colors polish!</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0q3kvswiy4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1jgvx9z</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>The gross green of my dreams</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgvx9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1jgvi3p</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Finally made my storage look nice</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgvi3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1jgunun</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>delightfully surprised by this polish</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s4157s1n4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1jgujmg</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>How are people’s experience with Abomination Cosmetics?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgujmg/how_are_peoples_experience_with_abomination/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1jgubm2</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Spring Nails ✨</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgubm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1jgu3ot</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce HHC Mother’s Day Duo</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgu3ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1jgu22u</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>An Unwhittleable Wishlist over Frozen Memories</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o9hoo465i4qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1jgu1jx</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>tuxedo approved shorties</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d28zqo9uh4qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1jgtz5r</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Spring Aura Nails</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgtz5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1jgthq4</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Remember when I said the China Glaze topcoat was decent?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgthq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1jgteq8</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Fairycore Spring 🌱 🪻</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgteq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1jgfu5a</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Reggae nails!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgfu5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1jgfywz</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>UK alternatives to Cirque Georgette?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgfywz/uk_alternatives_to_cirque_georgette/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1jgsq1n</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>New Favourite Combo!! 🐞🐞</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do9y4zvq64qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1jgrjpl</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>How are we feeling about Sassy Sauce’s “Here Kitty Kitty?”</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4wmaess1y3qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1jgq1qn</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>☘️Late to the Shake Your Shamrock Party☘️</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgq1qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1jgpt2k</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Well I decided to join the cool kids...</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgpt2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1jgpnpz</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Now playing: Dark Blue by Jack’s Mannequin</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgpnpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1jgplkk</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Is it possible to preserve the thermal effect on thermal polishes, or is it inevitable that they die eventually?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgplkk/is_it_possible_to_preserve_the_thermal_effect_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1jgp598</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Stiff, hard nails; constant snapping</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgp598/stiff_hard_nails_constant_snapping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1jgp0q9</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>How to stop bubbling with magnetics?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgp0q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1jgoxrw</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>How do we feel about LynBDesigns?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgoxrw/how_do_we_feel_about_lynbdesigns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1jgovt7</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Did people wear white nail polish in the 80s?</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgovt7/did_people_wear_white_nail_polish_in_the_80s/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1jgos3p</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>first ever cirque colors haul</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ta2hws66d3qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1jgofri</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Spring calls for pastel rainbows</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgofri</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1jgo1bk</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Seche vite and toluene (TW)</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgo1bk/seche_vite_and_toluene_tw/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1jgnqrz</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>nail polish pulling back?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0pr2wyg53qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1jgna1d</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Pls help me 3 broken nails</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgna1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1jgn7ff</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>This color combo is just *chef's kiss*</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgn7ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1jgmpyg</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Neon french for spring</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blnj7v9tx2qe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1jgmkyi</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>lavender / gold ✨️</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgmkyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1jglvrl</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Cupcake Polish Easter Collection</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goc97cqsr2qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1jglpzz</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>What shades best match the green wall in Severance?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jglpzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1jglb6k</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Gel Polish Dupe?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9pk4va4jn2qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1jgl33t</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>[DISO]-Bee’s Knees Lacquer: Who you gonna call?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4149pv7vl2qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1jgk2ry</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>what top coat for holographic formulas????</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgk2ry/what_top_coat_for_holographic_formulas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1jgjzj7</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Took way too long to discover Clionadh</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgjzj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1jgjzds</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Please share: Your favorite press-ons, go!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgjzds/please_share_your_favorite_pressons_go/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1jgjxdi</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Trying to find a good "jelly" nail polish, any suggestions?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgjxdi/trying_to_find_a_good_jelly_nail_polish_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1jgju5f</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Help me decide !</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgju5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1jgjosl</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Well. This is new.</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgjosl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1jgixpd</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Is there any way to get this effect with lacquer? Magnetic and jelly combo?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pmcbwye6xpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1jgirkq</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>this polish is Just My Type</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2qek1g5g42qe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1jgiirc</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Getting even nail primer’s staying power!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgiirc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1jgiej7</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Turquoise stone mani</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgiej7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1jgi60e</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Squishy jelly goodness</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u242olqnz1qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1jghwrs</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Fields of Elysium</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jghwrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1jghrjo</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Can you help me find an alternative?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jghrjo/can_you_help_me_find_an_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1jghbns</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Attn: Holo Taco Canadian customers!</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azir3rgws1qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1jgh341</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>In love with this color but I feel like it clashes?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qoj6gdwuq1qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1jggv4d</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>13 years old nail polish.</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jggv4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1jgg6lb</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Is it Spring yet? 🌷</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgg6lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1jgfvzk</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | HHC : Sure Burt</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgfvzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1jgf53r</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>What nail polish thinner would you recommend?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgf53r/what_nail_polish_thinner_would_you_recommend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1jfvz1b</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>first day of spring, but i'm forever an autumn girlie!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qml5rqk72wpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1jgct78</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Milk tea flakie love</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgct78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1jh03wm</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Purple and Gold Kitty Cats plus Blep</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhndwu1516qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1jgzx2h</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Sets I did at school this week 💅🏽✨💖</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgzx2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1jgwyr6</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Fiancé picked my set again</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udshtt8z65qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1jguaqh</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Spring Nails ✨</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jguaqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1jgpx4b</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>"Swearing doesn't make you cool" - Omni-Invincible Fanart</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgpx4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1jgp3rc</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Spring design</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6cex26mf3qe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1jgokvp</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Metal charms/chains in nail art</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jgokvp/metal_charmschains_in_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1jgojcw</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I was inspired by a post and realized none of my boards were magnetic but my coffee table is.</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jbe62kneb3qe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1jgn8y0</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Taiwanese wedding set for my friend 😁</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfeyk26q13qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1jgn5cs</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I just got into making press ons and I'm in love</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgn5cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1jglajc</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>First design that my 55-year-old mother makes, how are you?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mvynmaen2qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1jgj393</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Pink perfection! 💅✨ Who else is obsessed?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgj393</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1jgicux</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Did my nails yesterday!💕</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jgicux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1jghuau</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dem9dy3x1qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1jggpvg</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Natural nails🥹</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x22bcceon1qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1jfx9tf</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Cherry red ❤️ what’s missing?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xzk3w2tbwpe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1jfy1sp</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>My Pokémon nail art 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jfy1sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1jg27tf</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>What else can be added to this design?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z64ewtoucxpe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1jgbv1j</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>💎 Ice Cold, but Make It Fashion ❄️✨</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wqmkrsu30qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar 23 08:10:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_23.xlsx
+++ b/data/collected_data/2025_03_23.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1297"/>
+  <dimension ref="A1:C1489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22482,6 +22482,3270 @@
         </is>
       </c>
     </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1jhu6ul</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>obsessed 🤩</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/owfe364naeqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1jhu4gk</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>I'm a beginner in nails, do you like them?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ji4cxfvq9eqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1jhu1y2</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Gel polish</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjnvvmds8eqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1jhu1la</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>i feel like eating them</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eftx2yyn8eqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1jhtyfd</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>New to doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhtyfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1jhtujx</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>OG Ruby Slippers 👠</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhtujx/og_ruby_slippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1jhtnkl</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>🍒 Pink Cherry Nails 🍒</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zirmzi0e3eqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1jhthoe</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>What would you do?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhthoe/what_would_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1jhswxz</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Chrome. That’s it.</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhswxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1jhsvyr</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Press-Ons Question!</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhsvyr/pressons_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1jhsqgk</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>I love a simple French mani</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/782ahpbdrdqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1jhsn8b</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>I am in love with gel builder.</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tewpibaqdqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1jhs793</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>What service should I ask for ?</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xx7tqsvqkdqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1jhsagn</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>I love ombré</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvj14yhtldqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1jhs556</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Stencil for nail art</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhs556/stencil_for_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1jhrz6m</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Did my own nails!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pm41u0n2idqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1jhksuh</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Am I overreacting</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhksuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1jhqbfw</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Best pastel yellow nail polish</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhqbfw/best_pastel_yellow_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1jhncc2</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>DIY Gel Nails</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhncc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1jhnshf</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Um.. is this right??</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhnshf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1jhoh55</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Advice: are these bad?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhoh55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1jhr5z2</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>💜 chrome &amp; glitter ✨</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwaeiq209dqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1jhqy3u</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>best gel polishes??</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhqy3u/best_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1jhqxpy</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Gel X fill on my SIL!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhqxpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1jhq3wn</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Recent hard gel overlays I’ve done on my clients natural nails</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhq3wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1jhq2ui</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Japan trip nails!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7ndtzsixcqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1jhpuha</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Ghost face nails I did a while back &lt;3</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxe7t1f6vcqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1jhpmc4</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Mis uñas naturales ❤️✨</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yftm3euwscqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1jhphms</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Orange nails!</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9pd8xdlrcqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1jhpg59</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Tried something new today</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhpg59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1jhp340</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>This is the first time I've fallen in love. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjlzqrjjncqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1jhopxc</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhopxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1jhonio</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Own coat nail polish</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhonio/own_coat_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1jhobbc</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>need a nail expert</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhobbc/need_a_nail_expert/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1jho5q0</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>My gal is amazing.</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m66q0nqkecqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1jhneu1</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Worked hard on these and wanted to show off, inspired by Kali Uchis</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhneu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1jho01f</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Ladies, help! Do we love these?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jho01f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1jhnslt</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>First full set</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhnslt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1jhnmky</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Should I have the salon fix them?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhnmky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1jhnkka</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Black and white matte</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/37slps539cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1jhnhkf</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Don Julio nails 🥃🤎</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhnhkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1jhneuo</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Sad!!!😭😭😭 It's time for a touch-up. What should I choose now?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvlfpgvl7cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1jhndih</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>What's in your bag?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgn5x4z87cqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1jhmo80</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Spring nails 💅</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9dw15fu0cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1jhn4zd</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Ballerina Gown is my go-to color 🩰</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/001u6hi05cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1jhmy7x</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Some Spring pastel flowers 😍</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxb79gpb3cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1jhmv0n</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Cute birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhmv0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1jhmsid</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>My nail girl ateee with this set.</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhmsid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1jhmc0w</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Let’s call this one ‘Angel Dust’ nails</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd2n5h5wxbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1jhm6x6</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Paid $75. Was I over charged?</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awb49xcmwbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1jhknrp</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhknrp/nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1jhiqo5</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>What are these white spots?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhiqo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1jhm4a6</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Strawberry 🍓 press ons!</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nbmkwgyvbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1jhlzbn</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>[OC] And this is how my nails looked after an hour and a half of manicure. Does anyone know what this effect is called?</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8e3jo7bpubqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1jhkxv8</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Going to be trying my hand at press ons, advice needed!</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhkxv8/going_to_be_trying_my_hand_at_press_ons_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1jhlt79</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Personally.. OBSESSED</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3q53kdatbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1jhlmxs</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Stepped outside my comfort zone and I L O V E it!</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuu3c1zsrbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1jhlb0l</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Is it not normal to touch your nail tech with your other fingers?</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhlb0l/is_it_not_normal_to_touch_your_nail_tech_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1jhl8y6</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Help I don't know what I'm asking for so I never get my nails done 😩</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhl8y6/help_i_dont_know_what_im_asking_for_so_i_never/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1jhkzr1</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>really loving this colour and the iridescent accents make me so happy 🥺🩵</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhkzr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1jhkrnf</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>first time at a private studio and I'm never going back to a salon!</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhkrnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1jhkgz5</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>cottagecore chic 🌿</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhkgz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1jhkbn3</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Had to bring the spring vibes!</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yp6tsnrgbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1jhk79e</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Spring is here 🌼</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0c5gh1rfbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1jhjziy</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Encapsulated Flowers by my Nail Girl</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhjziy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1jhjx71</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Sick of painting my nails so I’m trying press ons for the first time 🙂</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58b3u53ddbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1jhjvu9</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/th1ofr21dbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1jhjnan</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Is it normal that I got charged $95 for this?</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhjnan</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1jhjefj</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Love a Fresh Mani</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhjefj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1jhj9gg</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Love this summer blue</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goroplgu7bqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1jhj12t</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>The cleanest set I’ve painted!</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhj12t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1jhix9x</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Midas touch</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iuddxf35bqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1jhhjsf</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Gel polish pooling off nails?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhhjsf/gel_polish_pooling_off_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1jhhoc9</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>“Babydoll Pink” Nail polish dupe</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhhoc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1jhiryt</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Help: Short nail solutions!</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyp3g1gu3bqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1jhiqv6</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Nails done by me 🥰 I'm crazy about this beautiful green 💚</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhiqv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1jhiacw</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhiacw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1jhhaxb</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>First time doing gel c</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhhaxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1jhh74p</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Some easter-y nails🐣🌷</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hulbrdu7raqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1jhh2dn</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>One of my favorite sets to date!!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awwx4mm6qaqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1jhgpxq</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Strawberry season is here! 🍓</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/podry82hnaqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1jhgm5m</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Help, are these supposed to be so arched?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhgm5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1jhglq9</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>💚 ILNP Highline 💛</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhglq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1jhfrjv</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Starting to feel like I’m getting the hang of doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzyidlq0gaqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1jhfj0o</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>First try with the adhesive press on style.</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vhk0gj5eaqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1jh6koj</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Infected nail bed</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jh6koj/infected_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1jh8zcl</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>What’s the perfect occasion for these nails? 🤔</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh8zcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1jh89uo</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Spring inspired nails 💅</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxs9a26yr8qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1jh1xwf</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>3 month nail journey</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh1xwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1jh1v1i</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80j4axc3l6qe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1jh9ouv</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>why is my gel top coat not drying?</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jh9ouv/why_is_my_gel_top_coat_not_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1jheo5a</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Nail glue recommendations</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1diuxjgh7aqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1jgxoko</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Nail Break</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc78226kd5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1jgpuwp</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Gel X beginner</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jgpuwp/gel_x_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1jgzagt</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Pinterest recreation</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yizu2140t5qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1jh0tfx</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what this is and/or why it happens. **Bonus points for advice to fix it**</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh0tfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1jh7eit</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Why are my nails like this and what can I do grow back the "flesh" beneath? It's been like this ever since. I'm cutting with scissors, no clip. (I'm male, grown my nails for emphasis to demonstrate on picture)</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lznxb7cfj8qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1jh9c3a</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Jinx (Arcane) inspired nails by me.</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh9c3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1jhels9</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>gel x help/advice/ best products for application?</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1jhels9/gel_x_helpadvice_best_products_for_application/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1jhe8xs</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Do y’all like my “cat nails” ?</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhe8xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1jhtq6x</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>OG Ruby Slippers 👠</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhtq6x/og_ruby_slippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1jhtecb</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Inspired by a post last week asking for polishes that cut/kill/slay/pretty much just own it, I put on the brightest polishes that I own. Seems that ILNP Vaperwave was the winner which I (unfortunately) don’t have but I did have some other honorable mentions….ILNP Summer kills it</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhtecb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1jhsvza</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Admitting defeat: what’s your routine for creating long, strong nails under regular lacquer ✨artifically✨</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhsvza/admitting_defeat_whats_your_routine_for_creating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1jhrp0k</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Help Finding a Kelly Green Shade (I think)</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhrp0k/help_finding_a_kelly_green_shade_i_think/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1jhrhqh</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Storage options</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhrhqh/storage_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1jhr6tx</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Nail tech cut the side of my cuticle with the nail drill</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhr6tx/nail_tech_cut_the_side_of_my_cuticle_with_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1jhr103</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>The many faces of BKL's "I Choose the Bear"</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhr103</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1jhqp6q</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Pruny fingers post-gel removal?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhqp6q/pruny_fingers_postgel_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1jhqc57</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Holo Taco shipping to Canada</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhqc57/holo_taco_shipping_to_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1jhpsc8</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Anybody know why some of Color Club’s holos are randomly $18.50 when all the rest are $14?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7yprrmlucqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1jhpd6j</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Emily de Molly- Current Events</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v2vu1hwaqcqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1jhp4ov</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Emily de Molly chipping easily?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhp4ov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1jhox4f</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Thanks to the person who was hating on crackle polish</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uj0smkxlcqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1jho2hf</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Clionadh Thermonuclear</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2lybm6nqdcqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1jhntwl</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Green Aura 💚</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lxcks5thbcqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1jhntk5</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Guess which finger has the dupe!😉😛🩵</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhntk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1jhn87w</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>ILNP - Blue Lagoon</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aa54ljp3cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1jhmpbt</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>robin's egg flakie for spring</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.imgur.com/a/TXFxfe5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1jhmpa6</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Welcome to Stardew Valley</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj4ic0iy0cqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1jhmnd1</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Anybody else pick up Holo Taco's Off The Deep End?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhmnd1/anybody_else_pick_up_holo_tacos_off_the_deep_end/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1jhmir7</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Haul or Nah for $20?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhmir7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1jhmamj</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Worth the wait. Lurid haul and protos</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eb4aryvjxbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1jhm4zf</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>what are your sassy sauce must haves? (besides cock a doodle doom ofc, that’s already in my cart 😇)</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhm4zf/what_are_your_sassy_sauce_must_haves_besides_cock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1jhm226</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>How do you keep track of which images you've already stamped?</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhm226/how_do_you_keep_track_of_which_images_youve/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1jhm1q8</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Polishes for cloudy days?</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhm1q8/polishes_for_cloudy_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1jhluqf</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Making my own galaxy themed nails!</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhluqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1jhlu8d</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>almond tea 💜🫖</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhlu8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1jhlhos</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>What brands make mini collection bottles?</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhlhos/what_brands_make_mini_collection_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1jhlepy</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Which top 5 polishes you currently own MAKE your collection?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwe6oiaupbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1jhlcoz</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Bluring base only</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5xq5wqdpbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1jhkxrd</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Broke my no-buy 🫠</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f678vjgzlbqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1jhkicp</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhkicp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1jhjs97</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>50 Shades of Greige + ☀️ = 🌈</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2b6nmrl9cbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1jhjns5</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Nails inspired by Buffy</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8qqryk5bbqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1jhiv82</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse + Sassy Sauce LSD 🥹✨</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhiv82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1jhis5y</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Regular polish!</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhis5y/regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1jhhymq</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Helping my inner teen😅</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhhymq/helping_my_inner_teen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1jhho4w</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>I’m blue 💙🦋</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhho4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1jhhnos</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>First Sassy Sauce Order!</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhhnos</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1jhhgj6</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Dupe request for Salamadria</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhhgj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1jhhdq0</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Blue/Green polish</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/jsf4d4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1jhhaf5</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>My favorite spring mani, with matching bracelet</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvtgynmvraqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1jhej9l</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Staying sane with first Mooncat haul - help</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhej9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1jhh4aa</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>It’s always Halloween in my heart!</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mtq5ce5lqaqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1jhf1nf</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>a lilac moment 💟💫✨</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5msq2efaaqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1jhh3an</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>New Candy Moyo colors at Dollar Tree</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhh2gw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1jhgnj8</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>💙💪Rosie the Riveter💛❤️</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhgnj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1jhgk6j</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>💚 ILNP Highline 💛</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhgk6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1jhg7sk</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Loving the new ILNP spring collection</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhg7sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1jhfxzn</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Looking for irregular flakies for franken polish. I can't find any!</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhfxzn/looking_for_irregular_flakies_for_franken_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1jhfkq9</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>The Scarlet Fox - BKL</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhfkq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1jhes8t</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Delusions/Illusions Collection Comparison - Cirque</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhes8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1jheqsr</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Best at-home thinner?</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jheqsr/best_athome_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1jheoqc</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Pastel Yellow? By Clionadh Cosmetics is so beautiful</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jheoqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1jhej7y</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>What are the ESSENTIAL toppers every collection should have?</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhej7y/what_are_the_essential_toppers_every_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1jhec0r</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Come Out To Socialize</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhec0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1jhdpjx</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Oh. Myyyy 😍😍 New favorite pink for me!</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhdpjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1jhcoe1</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Problems with Orly?</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhcoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1jhbxg3</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Starfire✨</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhbxg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1jhbe6e</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>At home gel polish</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrgdhcf3i9qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1jhax0n</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>twin peaks - has anyone made a collection inspired by the peaks?</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jhax0n/twin_peaks_has_anyone_made_a_collection_inspired/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1jh9brh</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Thermals with Long Nails 😍</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh9brh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1jh8f6c</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>How to improve these shitty nails..🤷🏻</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w2ft0abt8qe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1jh89ea</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Love a green 💚</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0khqg6ztr8qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1jh7u36</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>First time trying 3D nail stickers</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2rzgvmmn8qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1jh7kba</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>La Petite Mort🩵🤍🧲</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh7kba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1jgvdof</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Orly nail bonder base coat alternatives?</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1djxv44t4qe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1jgyztj</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Top and Base coat recommendations</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jgyztj/top_and_base_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1jh01zw</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Ideas for labeling thermal polish bottles to see both transition colors</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1jh01zw/ideas_for_labeling_thermal_polish_bottles_to_see/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1jh5hjn</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Digitalis 💅</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kg9mz87x7qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1jh410e</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>Please tell me I can buy Moth in the US</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh410e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1jhu2ug</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>My January snake nails 🐍</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhu2ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1jhu204</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>from this week</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhu204</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1jhtnse</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>🍒 Pink Cherry Nails 🍒</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vlibewg3eqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1jhrmbl</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>Is stamping gel the same as nail art gel?</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jhrmbl/is_stamping_gel_the_same_as_nail_art_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1jhqpgp</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>My March spring set :)</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhqpgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1jhqfv9</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>Can we just look at this 😱✨❤️</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e0efdvw41dqe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1jhprj4</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>It took me hours for my 12-year-old baby ❤️🐅</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1el2l1eucqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1jhoqv2</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhoqv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1jhiwrc</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Midas touch</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md6lshzy4bqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1jhimc9</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Honestly, what do you think of these nails? Should I improve anything? 😅</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zka8n1ai2bqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1jhhvg1</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Any suggestions on what to do different with the left hand lol</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sujqwxyfwaqe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1jhh3jq</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Favorite Kraft Heinz brands</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhh3jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1jhf6qc</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Sencillas, elegantes y con mucho estilo ✨ ¿Qué opinan?</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzlhwc95baqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1jhewiu</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Pinterest recreation</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inc8yeza9aqe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1jhctkh</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czme54ddt9qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1jhbn89</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Bad bunny inspired</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49m7zqr3k9qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1jh3aj3</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Show &amp; Tell... Nail Edition 😉💅</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh3aj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1jhau7b</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>3D Forest Nature Nails🍃🐞</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jhau7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1jh7sq5</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>what can i use?</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1jh7sq5/what_can_i_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1jh7m4q</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>Spring Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d8hmgukl8qe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1jh5ave</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>what is this product?</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1jh5ave</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>